<commit_message>
Process with tested project root
</commit_message>
<xml_diff>
--- a/Config/Popular_Credentials.xlsx
+++ b/Config/Popular_Credentials.xlsx
@@ -104,9 +104,6 @@
     <t>http://dmsconnect.maruti.com/</t>
   </si>
   <si>
-    <t>aarathy.nair@quadance.com;yedu.yesodharan@quadance.com;mafna.janeefar@quadance.com</t>
-  </si>
-  <si>
     <t>ServiceTesting SDWan</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>DMS Time Out</t>
+  </si>
+  <si>
+    <t>yedu.yesodharan@quadance.com;mafna.janeefar@quadance.com</t>
   </si>
 </sst>
 </file>
@@ -471,8 +471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T13" sqref="T13"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,7 +503,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -521,13 +521,13 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" t="s">
         <v>30</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
       </c>
       <c r="K1" t="s">
         <v>12</v>
@@ -542,13 +542,13 @@
         <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P1" t="s">
         <v>21</v>
       </c>
       <c r="Q1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R1" t="s">
         <v>22</v>
@@ -565,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -589,7 +589,7 @@
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>16</v>
@@ -607,16 +607,16 @@
         <v>6</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="Q2">
         <v>70</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>25</v>

</xml_diff>